<commit_message>
finish functioning excel file export
</commit_message>
<xml_diff>
--- a/docs/excel-reports/Birthday_Party_2025-04-18.xlsx
+++ b/docs/excel-reports/Birthday_Party_2025-04-18.xlsx
@@ -8,12 +8,15 @@
   <sheets>
     <sheet name="Expenses" r:id="rId3" sheetId="1"/>
     <sheet name="Consumers" r:id="rId4" sheetId="2"/>
+    <sheet name="Category Summary" r:id="rId5" sheetId="3"/>
+    <sheet name="Participants Balance" r:id="rId6" sheetId="4"/>
+    <sheet name="Debts" r:id="rId7" sheetId="5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
   <si>
     <t>Amount Paid</t>
   </si>
@@ -46,6 +49,39 @@
   </si>
   <si>
     <t>Transportation</t>
+  </si>
+  <si>
+    <t>Raw cost</t>
+  </si>
+  <si>
+    <t>Adjust Cost</t>
+  </si>
+  <si>
+    <t>Per Consumer</t>
+  </si>
+  <si>
+    <t>Total Participation Fee</t>
+  </si>
+  <si>
+    <t>Total Consumed</t>
+  </si>
+  <si>
+    <t>Total Expense</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Even</t>
+  </si>
+  <si>
+    <t>Debtor</t>
+  </si>
+  <si>
+    <t>Creditor</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -219,4 +255,275 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="13.25390625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.515625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.21484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.8359375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="5.25390625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="20.13671875" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>150.0</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>50.0</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>200.0</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>90.0</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>135.0</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>45.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>180.0</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>45.0</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>135.0</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>45.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>60.0</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>10.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="15.015625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="12.921875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="7.7265625" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>115.0</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>200.0</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>85.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>115.0</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>-15.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>250.0</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>150.0</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>-100.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>50.0</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>-10.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="6.984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="8.03515625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.8828125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>10.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>